<commit_message>
system design cheat sheet
</commit_message>
<xml_diff>
--- a/misc/src/main/resources/systemdesign/SystemDesignCheatSheet.xlsx
+++ b/misc/src/main/resources/systemdesign/SystemDesignCheatSheet.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/georgy.saukov/Desktop/dev/training/java-machine/misc/src/main/resources/systemdesign/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40BD6013-E197-8C4C-A358-DBFF4F82A56C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1CEF764-581D-8A4E-8C97-3548805F5273}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="43060" yWindow="1640" windowWidth="27640" windowHeight="16940" xr2:uid="{62866BA2-04DA-2641-9EBD-EF47019D4137}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="35840" windowHeight="20340" xr2:uid="{62866BA2-04DA-2641-9EBD-EF47019D4137}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="SystemCheatSheet" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="98">
   <si>
     <t>Database architecture &amp; design </t>
   </si>
@@ -79,23 +80,6 @@
   </si>
   <si>
     <t>federation (split DB by use case users. Order etc, )</t>
-  </si>
-  <si>
-    <t>BASE</t>
-  </si>
-  <si>
-    <r>
-      <t>Basically available</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="16"/>
-        <color rgb="FF24292E"/>
-        <rFont val="Helvetica"/>
-        <family val="2"/>
-      </rPr>
-      <t> </t>
-    </r>
   </si>
   <si>
     <t>SQL tuning</t>
@@ -313,13 +297,37 @@
   </si>
   <si>
     <t>PostressSQL</t>
+  </si>
+  <si>
+    <t>Basically available </t>
+  </si>
+  <si>
+    <t>BASE principle</t>
+  </si>
+  <si>
+    <t>RDBMS implementations:</t>
+  </si>
+  <si>
+    <t>NOSQL implementations:</t>
+  </si>
+  <si>
+    <t>Cluster replications</t>
+  </si>
+  <si>
+    <t>Store types:</t>
+  </si>
+  <si>
+    <t>desription:</t>
+  </si>
+  <si>
+    <t>--</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -328,46 +336,90 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="13"/>
+      <sz val="12"/>
       <color rgb="FF1D2228"/>
       <name val="Helvetica Neue"/>
       <family val="2"/>
     </font>
     <font>
-      <sz val="16"/>
+      <sz val="12"/>
       <color rgb="FF24292E"/>
       <name val="Helvetica"/>
       <family val="2"/>
     </font>
     <font>
-      <sz val="16"/>
+      <b/>
+      <sz val="12"/>
       <color rgb="FF24292E"/>
-      <name val="Helvetica"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="16"/>
-      <color rgb="FF6A737D"/>
       <name val="Helvetica"/>
       <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="16"/>
+      <color rgb="FF1D2228"/>
+      <name val="Helvetica Neue"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="14"/>
       <color rgb="FF24292E"/>
       <name val="Helvetica"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color rgb="FF24292E"/>
+      <name val="Helvetica"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color rgb="FF24292E"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color rgb="FF24292E"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -375,19 +427,177 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -703,406 +913,533 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{66396D0F-A29D-4549-A6CA-414560F56E87}">
-  <dimension ref="A2:F55"/>
+  <dimension ref="A2:E58"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="E28" sqref="E28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="52.1640625" customWidth="1"/>
-    <col min="2" max="2" width="37.6640625" customWidth="1"/>
-    <col min="3" max="3" width="66.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="24" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="52.1640625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="50.6640625" style="2" customWidth="1"/>
+    <col min="3" max="3" width="66.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="24" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="16384" width="10.83203125" style="2"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A2" s="1" t="s">
+    <row r="2" spans="1:5" ht="20" x14ac:dyDescent="0.2">
+      <c r="A2" s="5" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B3" t="s">
+    <row r="3" spans="1:5" ht="19" x14ac:dyDescent="0.25">
+      <c r="A3" s="12" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" ht="21" x14ac:dyDescent="0.25">
-      <c r="B4" t="s">
+      <c r="B3" s="12"/>
+      <c r="C3" s="12"/>
+    </row>
+    <row r="4" spans="1:5" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="B4" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="D4" t="s">
+      <c r="C4" s="18" t="s">
+        <v>92</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="16"/>
+      <c r="B5" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" s="14" t="s">
+        <v>57</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="16"/>
+      <c r="B6" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6" s="14" t="s">
+        <v>58</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="17"/>
+      <c r="B7" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="C7" s="14" t="s">
+        <v>89</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="19" x14ac:dyDescent="0.25">
+      <c r="A8" s="11"/>
+      <c r="B8" s="9"/>
+      <c r="C8" s="9"/>
+      <c r="E8" s="3" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="23" t="s">
+        <v>13</v>
+      </c>
+      <c r="B9" s="21" t="s">
+        <v>15</v>
+      </c>
+      <c r="C9" s="22"/>
+      <c r="E9" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="24"/>
+      <c r="B10" s="21" t="s">
+        <v>16</v>
+      </c>
+      <c r="C10" s="22"/>
+      <c r="E10" s="3" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="25"/>
+      <c r="B11" s="21" t="s">
+        <v>17</v>
+      </c>
+      <c r="C11" s="22"/>
+      <c r="E11" s="3" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="19" x14ac:dyDescent="0.25">
+      <c r="A12" s="6"/>
+      <c r="C12" s="7"/>
+      <c r="E12" s="3" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="18" x14ac:dyDescent="0.2">
+      <c r="A13" s="26" t="s">
+        <v>18</v>
+      </c>
+      <c r="B13" s="29" t="s">
+        <v>19</v>
+      </c>
+      <c r="C13" s="30"/>
+      <c r="D13" s="4" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="18" x14ac:dyDescent="0.2">
+      <c r="A14" s="27"/>
+      <c r="B14" s="29" t="s">
         <v>59</v>
       </c>
-      <c r="E4" s="5" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" ht="21" x14ac:dyDescent="0.25">
-      <c r="C5" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D5" t="s">
+      <c r="C14" s="30"/>
+      <c r="E14" s="3" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="18" x14ac:dyDescent="0.2">
+      <c r="A15" s="28"/>
+      <c r="B15" s="29" t="s">
+        <v>20</v>
+      </c>
+      <c r="C15" s="30"/>
+      <c r="E15" s="3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="18" x14ac:dyDescent="0.2">
+      <c r="A16" s="9"/>
+      <c r="B16" s="10"/>
+      <c r="C16" s="9"/>
+      <c r="E16" s="3" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="19" x14ac:dyDescent="0.25">
+      <c r="A17" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="B17" s="12"/>
+      <c r="C17" s="12"/>
+      <c r="E17" s="3" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="18" x14ac:dyDescent="0.2">
+      <c r="A18" s="31" t="s">
+        <v>91</v>
+      </c>
+      <c r="B18" s="20" t="s">
+        <v>90</v>
+      </c>
+      <c r="C18" s="34" t="s">
+        <v>21</v>
+      </c>
+      <c r="E18" s="3" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="32"/>
+      <c r="B19" s="20" t="s">
+        <v>22</v>
+      </c>
+      <c r="C19" s="35"/>
+      <c r="E19" s="3" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="33"/>
+      <c r="B20" s="20" t="s">
+        <v>23</v>
+      </c>
+      <c r="C20" s="36"/>
+      <c r="E20" s="3" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" ht="19" x14ac:dyDescent="0.25">
+      <c r="A21" s="6"/>
+      <c r="B21" s="7"/>
+      <c r="C21" s="7"/>
+      <c r="D21" s="4" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" ht="19" x14ac:dyDescent="0.25">
+      <c r="A22" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="B22" s="29" t="s">
+        <v>94</v>
+      </c>
+      <c r="C22" s="30"/>
+      <c r="E22" s="3" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" ht="19" x14ac:dyDescent="0.25">
+      <c r="A23" s="6"/>
+      <c r="B23" s="7"/>
+      <c r="C23" s="7"/>
+      <c r="E23" s="3" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" ht="19" x14ac:dyDescent="0.25">
+      <c r="A24" s="37" t="s">
+        <v>95</v>
+      </c>
+      <c r="B24" s="38" t="s">
+        <v>96</v>
+      </c>
+      <c r="C24" s="38" t="s">
+        <v>93</v>
+      </c>
+      <c r="E24" s="3" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" ht="19" x14ac:dyDescent="0.25">
+      <c r="A25" s="19" t="s">
+        <v>24</v>
+      </c>
+      <c r="B25" s="39" t="s">
+        <v>25</v>
+      </c>
+      <c r="C25" s="39" t="s">
+        <v>26</v>
+      </c>
+      <c r="E25" s="3" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" ht="19" x14ac:dyDescent="0.25">
+      <c r="A26" s="39" t="s">
+        <v>27</v>
+      </c>
+      <c r="B26" s="39" t="s">
+        <v>28</v>
+      </c>
+      <c r="C26" s="39" t="s">
+        <v>29</v>
+      </c>
+      <c r="E26" s="3" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" ht="19" x14ac:dyDescent="0.25">
+      <c r="A27" s="19" t="s">
+        <v>30</v>
+      </c>
+      <c r="B27" s="39" t="s">
+        <v>31</v>
+      </c>
+      <c r="C27" s="39" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" ht="19" x14ac:dyDescent="0.25">
+      <c r="A28" s="19" t="s">
+        <v>33</v>
+      </c>
+      <c r="B28" s="40" t="s">
+        <v>97</v>
+      </c>
+      <c r="C28" s="40" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" ht="18" x14ac:dyDescent="0.2">
+      <c r="B29" s="7"/>
+      <c r="C29" s="7"/>
+    </row>
+    <row r="30" spans="1:5" ht="18" x14ac:dyDescent="0.2">
+      <c r="B30" s="7"/>
+      <c r="C30" s="7"/>
+    </row>
+    <row r="31" spans="1:5" ht="18" x14ac:dyDescent="0.2">
+      <c r="B31" s="7"/>
+      <c r="C31" s="7"/>
+    </row>
+    <row r="32" spans="1:5" ht="18" x14ac:dyDescent="0.2">
+      <c r="B32" s="7"/>
+      <c r="C32" s="7"/>
+    </row>
+    <row r="35" spans="1:4" ht="20" x14ac:dyDescent="0.2">
+      <c r="A35" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="B35" s="42" t="s">
         <v>60</v>
       </c>
-      <c r="F5" s="4" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" ht="21" x14ac:dyDescent="0.25">
-      <c r="C6" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D6" t="s">
-        <v>91</v>
-      </c>
-      <c r="F6" s="4" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" ht="21" x14ac:dyDescent="0.25">
-      <c r="C7" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="F7" s="4" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" ht="21" x14ac:dyDescent="0.25">
-      <c r="C8" s="2"/>
-      <c r="F8" s="4" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" ht="21" x14ac:dyDescent="0.25">
-      <c r="B9" t="s">
-        <v>13</v>
-      </c>
-      <c r="F9" s="4" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" ht="21" x14ac:dyDescent="0.25">
-      <c r="C10" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="F10" s="4" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" ht="21" x14ac:dyDescent="0.25">
-      <c r="C11" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="F11" s="4" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" ht="21" x14ac:dyDescent="0.25">
-      <c r="C12" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="F12" s="4" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" ht="21" x14ac:dyDescent="0.25">
-      <c r="B13" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="C13" s="2"/>
-      <c r="E13" s="5" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" ht="21" x14ac:dyDescent="0.25">
-      <c r="B14" s="2"/>
-      <c r="C14" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="F14" s="4" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" ht="21" x14ac:dyDescent="0.25">
-      <c r="B15" s="2"/>
-      <c r="C15" s="2" t="s">
+      <c r="C35" s="42"/>
+    </row>
+    <row r="36" spans="1:4" ht="68" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A36" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B36" s="42" t="s">
         <v>61</v>
       </c>
-      <c r="F15" s="4" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" ht="21" x14ac:dyDescent="0.25">
-      <c r="B16" s="2"/>
-      <c r="C16" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="F16" s="4" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" ht="21" x14ac:dyDescent="0.25">
-      <c r="B17" t="s">
-        <v>8</v>
-      </c>
-      <c r="F17" s="4" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" ht="21" x14ac:dyDescent="0.25">
-      <c r="B18" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="C18" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="D18" t="s">
-        <v>23</v>
-      </c>
-      <c r="F18" s="4" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" ht="21" x14ac:dyDescent="0.25">
-      <c r="C19" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="F19" s="4" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" ht="21" x14ac:dyDescent="0.25">
-      <c r="C20" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="F20" s="4" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" ht="21" x14ac:dyDescent="0.25">
-      <c r="C21" s="2"/>
-      <c r="E21" s="5" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" ht="21" x14ac:dyDescent="0.25">
-      <c r="B22" t="s">
-        <v>26</v>
-      </c>
-      <c r="C22" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="D22" t="s">
-        <v>28</v>
-      </c>
-      <c r="F22" s="4" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" ht="21" x14ac:dyDescent="0.25">
-      <c r="B23" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="C23" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="D23" t="s">
-        <v>31</v>
-      </c>
-      <c r="F23" s="4" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" ht="21" x14ac:dyDescent="0.25">
-      <c r="B24" t="s">
-        <v>32</v>
-      </c>
-      <c r="C24" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="D24" t="s">
-        <v>34</v>
-      </c>
-      <c r="F24" s="4" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" ht="21" x14ac:dyDescent="0.25">
-      <c r="B25" t="s">
-        <v>35</v>
-      </c>
-      <c r="F25" s="4" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" ht="21" x14ac:dyDescent="0.25">
-      <c r="F26" s="4" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A32" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B32" t="s">
+      <c r="C36" s="42"/>
+      <c r="D36" s="8"/>
+    </row>
+    <row r="37" spans="1:4" ht="43" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A37" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B37" s="41" t="s">
+        <v>66</v>
+      </c>
+      <c r="C37" s="41"/>
+    </row>
+    <row r="38" spans="1:4" ht="20" x14ac:dyDescent="0.2">
+      <c r="A38" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B38" s="42" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="33" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A33" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B33" t="s">
+      <c r="C38" s="42"/>
+    </row>
+    <row r="39" spans="1:4" ht="70" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A39" s="1"/>
+      <c r="B39" s="41" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="34" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A34" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B34" t="s">
+      <c r="C39" s="41"/>
+    </row>
+    <row r="40" spans="1:4" ht="19" x14ac:dyDescent="0.25">
+      <c r="A40" s="1"/>
+      <c r="B40" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="C40" s="6"/>
+    </row>
+    <row r="41" spans="1:4" ht="19" x14ac:dyDescent="0.25">
+      <c r="A41" s="1"/>
+      <c r="B41" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="C41" s="6"/>
+    </row>
+    <row r="42" spans="1:4" ht="19" x14ac:dyDescent="0.25">
+      <c r="A42" s="1"/>
+      <c r="B42" s="6"/>
+      <c r="C42" s="6"/>
+    </row>
+    <row r="43" spans="1:4" ht="21" x14ac:dyDescent="0.25">
+      <c r="A43" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B43" s="6" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="35" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A35" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B35" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" ht="68" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="1"/>
-      <c r="B36" s="6" t="s">
-        <v>65</v>
-      </c>
-      <c r="C36" s="6"/>
-      <c r="D36" s="6"/>
-    </row>
-    <row r="37" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A37" s="1"/>
-      <c r="B37" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A38" s="1"/>
-      <c r="B38" t="s">
+      <c r="C43" s="6" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="39" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A39" s="1"/>
-    </row>
-    <row r="40" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A40" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B40" t="s">
+    <row r="44" spans="1:4" ht="19" x14ac:dyDescent="0.25">
+      <c r="B44" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="C44" s="6" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" ht="19" x14ac:dyDescent="0.25">
+      <c r="B45" s="6" t="s">
         <v>70</v>
       </c>
-      <c r="C40" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B41" t="s">
-        <v>71</v>
-      </c>
-      <c r="C41" t="s">
+      <c r="C45" s="6" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" ht="19" x14ac:dyDescent="0.25">
+      <c r="B46" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="C46" s="6"/>
+    </row>
+    <row r="47" spans="1:4" ht="19" x14ac:dyDescent="0.25">
+      <c r="B47" s="6" t="s">
+        <v>87</v>
+      </c>
+      <c r="C47" s="6"/>
+    </row>
+    <row r="48" spans="1:4" ht="19" x14ac:dyDescent="0.25">
+      <c r="B48" s="6"/>
+      <c r="C48" s="6"/>
+    </row>
+    <row r="49" spans="1:3" ht="19" x14ac:dyDescent="0.25">
+      <c r="B49" s="6" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B42" t="s">
-        <v>72</v>
-      </c>
-      <c r="C42" t="s">
+      <c r="C49" s="6" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" ht="19" x14ac:dyDescent="0.25">
+      <c r="B50" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="C50" s="6" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" ht="19" x14ac:dyDescent="0.25">
+      <c r="B51" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="C51" s="6" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" ht="19" x14ac:dyDescent="0.25">
+      <c r="B52" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="C52" s="6" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B43" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B44" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B46" t="s">
-        <v>75</v>
-      </c>
-      <c r="C46" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B47" t="s">
-        <v>76</v>
-      </c>
-      <c r="C47" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B48" t="s">
+    <row r="53" spans="1:3" ht="19" x14ac:dyDescent="0.25">
+      <c r="B53" s="6" t="s">
         <v>77</v>
       </c>
-      <c r="C48" t="s">
+      <c r="C53" s="6" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" ht="19" x14ac:dyDescent="0.25">
+      <c r="B54" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="C54" s="6"/>
+    </row>
+    <row r="55" spans="1:3" ht="19" x14ac:dyDescent="0.25">
+      <c r="B55" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="C55" s="6"/>
+    </row>
+    <row r="56" spans="1:3" ht="19" x14ac:dyDescent="0.25">
+      <c r="B56" s="6" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B49" t="s">
-        <v>78</v>
-      </c>
-      <c r="C49" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B50" t="s">
-        <v>79</v>
-      </c>
-      <c r="C50" t="s">
+      <c r="C56" s="6"/>
+    </row>
+    <row r="57" spans="1:3" ht="19" x14ac:dyDescent="0.25">
+      <c r="B57" s="6"/>
+      <c r="C57" s="6"/>
+    </row>
+    <row r="58" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+      <c r="A58" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B58" s="6" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B51" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B52" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B53" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="55" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A55" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B55" t="s">
-        <v>90</v>
-      </c>
+      <c r="C58" s="6"/>
     </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="B36:D36"/>
+  <mergeCells count="19">
+    <mergeCell ref="B39:C39"/>
+    <mergeCell ref="B35:C35"/>
+    <mergeCell ref="B36:C36"/>
+    <mergeCell ref="B37:C37"/>
+    <mergeCell ref="B38:C38"/>
+    <mergeCell ref="A3:C3"/>
+    <mergeCell ref="A4:A7"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="A9:A11"/>
+    <mergeCell ref="A13:A15"/>
+    <mergeCell ref="B13:C13"/>
+    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="A17:C17"/>
+    <mergeCell ref="A18:A20"/>
+    <mergeCell ref="C18:C20"/>
+    <mergeCell ref="B22:C22"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F4343913-5B90-2D4B-BFC8-90ABE70DB230}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>